<commit_message>
added check for champions
</commit_message>
<xml_diff>
--- a/Datasetsets shared/missing training reports.xlsx
+++ b/Datasetsets shared/missing training reports.xlsx
@@ -235,7 +235,7 @@
     <t>B</t>
   </si>
   <si>
-    <t>Coffee Champions - ToT 1, HOR 1</t>
+    <t>HOR 1, Coffee Champions - ToT 1</t>
   </si>
   <si>
     <t>Coffee Champions - ToT 1</t>
@@ -244,13 +244,13 @@
     <t>HOR 1</t>
   </si>
   <si>
-    <t>Coffee Champions - ToT 1, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Village Champions</t>
-  </si>
-  <si>
-    <t>CATs / Agriculture Champions, WASH Champions Training, Coffee Champions - ToT 1, Village Champions, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
-  </si>
-  <si>
-    <t>Coffee Champions - ToT 1, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Village Champions, HOR 1</t>
+    <t>HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Coffee Champions - ToT 1, Village Champions</t>
+  </si>
+  <si>
+    <t>WASH Champions Training, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Village Champions, Coffee Champions - ToT 1, CATs / Agriculture Champions</t>
+  </si>
+  <si>
+    <t>HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, HOR 1, Coffee Champions - ToT 1, Village Champions</t>
   </si>
   <si>
     <t>Rugarama</t>

</xml_diff>

<commit_message>
check 11 for Rakai
</commit_message>
<xml_diff>
--- a/Datasetsets shared/missing training reports.xlsx
+++ b/Datasetsets shared/missing training reports.xlsx
@@ -244,13 +244,13 @@
     <t>HOR 1, Coffee Champions - ToT 1</t>
   </si>
   <si>
-    <t>Village Champions, Coffee Champions - ToT 1, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
-  </si>
-  <si>
-    <t>CATs / Agriculture Champions, Village Champions, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, WASH Champions Training, Coffee Champions - ToT 1</t>
-  </si>
-  <si>
-    <t>HOR 1, Village Champions, Coffee Champions - ToT 1, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
+    <t>Village Champions, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Coffee Champions - ToT 1</t>
+  </si>
+  <si>
+    <t>WASH Champions Training, Village Champions, Coffee Champions - ToT 1, CATs / Agriculture Champions, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
+  </si>
+  <si>
+    <t>Village Champions, HOR 1, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Coffee Champions - ToT 1</t>
   </si>
   <si>
     <t>HOR 3</t>

</xml_diff>

<commit_message>
check #11 on 31/3/2025
</commit_message>
<xml_diff>
--- a/Datasetsets shared/missing training reports.xlsx
+++ b/Datasetsets shared/missing training reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="71">
   <si>
     <t>district_name</t>
   </si>
@@ -49,15 +49,6 @@
     <t>Bujumiro_B</t>
   </si>
   <si>
-    <t>Kagorogoro_A</t>
-  </si>
-  <si>
-    <t>Kagorogoro_B</t>
-  </si>
-  <si>
-    <t>Kahenda</t>
-  </si>
-  <si>
     <t>Kanyamburara</t>
   </si>
   <si>
@@ -73,12 +64,6 @@
     <t>Karubuguma_2</t>
   </si>
   <si>
-    <t>Kemihoko_A</t>
-  </si>
-  <si>
-    <t>Kemihoko_B</t>
-  </si>
-  <si>
     <t>Kyarubingo</t>
   </si>
   <si>
@@ -91,21 +76,12 @@
     <t>Muyenga_TC</t>
   </si>
   <si>
-    <t>Nganiko_1</t>
-  </si>
-  <si>
     <t>Nganiko_2</t>
   </si>
   <si>
     <t>Nganiko_3</t>
   </si>
   <si>
-    <t>Nganiko_Central</t>
-  </si>
-  <si>
-    <t>Nganiko_TC</t>
-  </si>
-  <si>
     <t>Nyabwina_Buhanda</t>
   </si>
   <si>
@@ -238,19 +214,7 @@
     <t>Coffee Champions - ToT 1</t>
   </si>
   <si>
-    <t>HOR 1</t>
-  </si>
-  <si>
-    <t>HOR 1, Coffee Champions - ToT 1</t>
-  </si>
-  <si>
-    <t>Village Champions, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Coffee Champions - ToT 1</t>
-  </si>
-  <si>
-    <t>WASH Champions Training, Village Champions, Coffee Champions - ToT 1, CATs / Agriculture Champions, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
-  </si>
-  <si>
-    <t>Village Champions, HOR 1, HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection, Coffee Champions - ToT 1</t>
+    <t>HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
   </si>
   <si>
     <t>HOR 3</t>
@@ -620,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -660,10 +624,10 @@
         <v>2025</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -677,10 +641,10 @@
         <v>2025</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -694,10 +658,10 @@
         <v>2025</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -711,10 +675,10 @@
         <v>2025</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -728,10 +692,10 @@
         <v>2025</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -745,10 +709,10 @@
         <v>2025</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -762,10 +726,10 @@
         <v>2025</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -779,10 +743,10 @@
         <v>2025</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -796,10 +760,10 @@
         <v>2025</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -813,10 +777,10 @@
         <v>2025</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -830,10 +794,10 @@
         <v>2025</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -847,10 +811,10 @@
         <v>2025</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -864,10 +828,10 @@
         <v>2025</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -881,10 +845,10 @@
         <v>2025</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -898,10 +862,10 @@
         <v>2025</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -915,10 +879,10 @@
         <v>2025</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -932,10 +896,10 @@
         <v>2025</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -949,15 +913,15 @@
         <v>2025</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
@@ -966,15 +930,15 @@
         <v>2025</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
@@ -983,15 +947,15 @@
         <v>2025</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -1000,15 +964,15 @@
         <v>2025</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
         <v>30</v>
@@ -1017,15 +981,15 @@
         <v>2025</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
@@ -1034,15 +998,15 @@
         <v>2025</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -1051,15 +1015,15 @@
         <v>2025</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
@@ -1068,15 +1032,15 @@
         <v>2025</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -1085,10 +1049,10 @@
         <v>2025</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1102,10 +1066,10 @@
         <v>2025</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1119,10 +1083,10 @@
         <v>2025</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1136,10 +1100,10 @@
         <v>2025</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1153,10 +1117,10 @@
         <v>2025</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1170,10 +1134,10 @@
         <v>2025</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1187,10 +1151,10 @@
         <v>2025</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1204,10 +1168,10 @@
         <v>2025</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1221,10 +1185,10 @@
         <v>2025</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1238,146 +1202,194 @@
         <v>2025</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>44</v>
       </c>
       <c r="C37">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37">
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
         <v>45</v>
       </c>
       <c r="C38">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F38" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
       </c>
       <c r="C39">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E39" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F39" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39">
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
         <v>47</v>
       </c>
       <c r="C40">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40">
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>48</v>
       </c>
       <c r="C41">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41">
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
       </c>
       <c r="C42">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D42" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E42" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42">
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
         <v>50</v>
       </c>
       <c r="C43">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G43">
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
         <v>51</v>
       </c>
       <c r="C44">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44">
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1391,16 +1403,16 @@
         <v>2024</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F45" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G45">
-        <v>146</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1414,16 +1426,16 @@
         <v>2024</v>
       </c>
       <c r="D46" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G46">
-        <v>62</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1437,16 +1449,16 @@
         <v>2024</v>
       </c>
       <c r="D47" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F47" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G47">
-        <v>109</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1460,16 +1472,16 @@
         <v>2024</v>
       </c>
       <c r="D48" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F48" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G48">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1483,16 +1495,16 @@
         <v>2024</v>
       </c>
       <c r="D49" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F49" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G49">
-        <v>96</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1506,16 +1518,16 @@
         <v>2024</v>
       </c>
       <c r="D50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50">
         <v>72</v>
-      </c>
-      <c r="E50" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" t="s">
-        <v>82</v>
-      </c>
-      <c r="G50">
-        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1529,16 +1541,16 @@
         <v>2024</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F51" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G51">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1552,16 +1564,16 @@
         <v>2024</v>
       </c>
       <c r="D52" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F52" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G52">
-        <v>46</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1575,16 +1587,16 @@
         <v>2024</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F53" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="G53">
-        <v>107</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1598,16 +1610,16 @@
         <v>2024</v>
       </c>
       <c r="D54" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F54" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="G54">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1621,199 +1633,15 @@
         <v>2024</v>
       </c>
       <c r="D55" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E55" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F55" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G55">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56">
-        <v>2024</v>
-      </c>
-      <c r="D56" t="s">
-        <v>72</v>
-      </c>
-      <c r="E56" t="s">
-        <v>79</v>
-      </c>
-      <c r="F56" t="s">
-        <v>82</v>
-      </c>
-      <c r="G56">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57">
-        <v>2024</v>
-      </c>
-      <c r="D57" t="s">
-        <v>72</v>
-      </c>
-      <c r="E57" t="s">
-        <v>79</v>
-      </c>
-      <c r="F57" t="s">
-        <v>80</v>
-      </c>
-      <c r="G57">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58">
-        <v>2024</v>
-      </c>
-      <c r="D58" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" t="s">
-        <v>79</v>
-      </c>
-      <c r="F58" t="s">
-        <v>81</v>
-      </c>
-      <c r="G58">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" t="s">
-        <v>66</v>
-      </c>
-      <c r="C59">
-        <v>2024</v>
-      </c>
-      <c r="D59" t="s">
-        <v>72</v>
-      </c>
-      <c r="E59" t="s">
-        <v>79</v>
-      </c>
-      <c r="F59" t="s">
-        <v>81</v>
-      </c>
-      <c r="G59">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" t="s">
-        <v>67</v>
-      </c>
-      <c r="C60">
-        <v>2024</v>
-      </c>
-      <c r="D60" t="s">
-        <v>72</v>
-      </c>
-      <c r="E60" t="s">
-        <v>79</v>
-      </c>
-      <c r="F60" t="s">
-        <v>81</v>
-      </c>
-      <c r="G60">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61">
-        <v>2024</v>
-      </c>
-      <c r="D61" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" t="s">
-        <v>79</v>
-      </c>
-      <c r="F61" t="s">
-        <v>80</v>
-      </c>
-      <c r="G61">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>69</v>
-      </c>
-      <c r="C62">
-        <v>2024</v>
-      </c>
-      <c r="D62" t="s">
-        <v>72</v>
-      </c>
-      <c r="E62" t="s">
-        <v>79</v>
-      </c>
-      <c r="F62" t="s">
-        <v>80</v>
-      </c>
-      <c r="G62">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63">
-        <v>2024</v>
-      </c>
-      <c r="D63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E63" t="s">
-        <v>79</v>
-      </c>
-      <c r="F63" t="s">
-        <v>82</v>
-      </c>
-      <c r="G63">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added summary codes for trainings
</commit_message>
<xml_diff>
--- a/Datasetsets shared/missing training reports.xlsx
+++ b/Datasetsets shared/missing training reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="70">
   <si>
     <t>district_name</t>
   </si>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>HHT 2 - Financial Literacy and VSLA and and Business Enterprise Selection</t>
-  </si>
-  <si>
-    <t>HOR 3</t>
   </si>
   <si>
     <t>Rugarama</t>
@@ -1221,11 +1218,8 @@
       <c r="D37" t="s">
         <v>64</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>67</v>
-      </c>
-      <c r="F37" t="s">
-        <v>68</v>
       </c>
       <c r="G37">
         <v>146</v>
@@ -1244,11 +1238,8 @@
       <c r="D38" t="s">
         <v>64</v>
       </c>
-      <c r="E38" t="s">
-        <v>67</v>
-      </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G38">
         <v>62</v>
@@ -1267,11 +1258,8 @@
       <c r="D39" t="s">
         <v>64</v>
       </c>
-      <c r="E39" t="s">
-        <v>67</v>
-      </c>
       <c r="F39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G39">
         <v>109</v>
@@ -1290,11 +1278,8 @@
       <c r="D40" t="s">
         <v>64</v>
       </c>
-      <c r="E40" t="s">
-        <v>67</v>
-      </c>
       <c r="F40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G40">
         <v>121</v>
@@ -1313,11 +1298,8 @@
       <c r="D41" t="s">
         <v>64</v>
       </c>
-      <c r="E41" t="s">
-        <v>67</v>
-      </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G41">
         <v>96</v>
@@ -1336,11 +1318,8 @@
       <c r="D42" t="s">
         <v>64</v>
       </c>
-      <c r="E42" t="s">
-        <v>67</v>
-      </c>
       <c r="F42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G42">
         <v>61</v>
@@ -1359,11 +1338,8 @@
       <c r="D43" t="s">
         <v>64</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>67</v>
-      </c>
-      <c r="F43" t="s">
-        <v>68</v>
       </c>
       <c r="G43">
         <v>81</v>
@@ -1382,11 +1358,8 @@
       <c r="D44" t="s">
         <v>64</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>67</v>
-      </c>
-      <c r="F44" t="s">
-        <v>68</v>
       </c>
       <c r="G44">
         <v>46</v>
@@ -1405,11 +1378,8 @@
       <c r="D45" t="s">
         <v>64</v>
       </c>
-      <c r="E45" t="s">
-        <v>67</v>
-      </c>
       <c r="F45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G45">
         <v>107</v>
@@ -1428,11 +1398,8 @@
       <c r="D46" t="s">
         <v>64</v>
       </c>
-      <c r="E46" t="s">
-        <v>67</v>
-      </c>
       <c r="F46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G46">
         <v>83</v>
@@ -1451,11 +1418,8 @@
       <c r="D47" t="s">
         <v>64</v>
       </c>
-      <c r="E47" t="s">
-        <v>67</v>
-      </c>
       <c r="F47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G47">
         <v>141</v>
@@ -1474,11 +1438,8 @@
       <c r="D48" t="s">
         <v>64</v>
       </c>
-      <c r="E48" t="s">
-        <v>67</v>
-      </c>
       <c r="F48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G48">
         <v>163</v>
@@ -1497,11 +1458,8 @@
       <c r="D49" t="s">
         <v>64</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>67</v>
-      </c>
-      <c r="F49" t="s">
-        <v>68</v>
       </c>
       <c r="G49">
         <v>140</v>
@@ -1520,11 +1478,8 @@
       <c r="D50" t="s">
         <v>64</v>
       </c>
-      <c r="E50" t="s">
-        <v>67</v>
-      </c>
       <c r="F50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G50">
         <v>72</v>
@@ -1543,11 +1498,8 @@
       <c r="D51" t="s">
         <v>64</v>
       </c>
-      <c r="E51" t="s">
-        <v>67</v>
-      </c>
       <c r="F51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G51">
         <v>74</v>
@@ -1566,11 +1518,8 @@
       <c r="D52" t="s">
         <v>64</v>
       </c>
-      <c r="E52" t="s">
-        <v>67</v>
-      </c>
       <c r="F52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G52">
         <v>97</v>
@@ -1589,11 +1538,8 @@
       <c r="D53" t="s">
         <v>64</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>67</v>
-      </c>
-      <c r="F53" t="s">
-        <v>68</v>
       </c>
       <c r="G53">
         <v>187</v>
@@ -1612,11 +1558,8 @@
       <c r="D54" t="s">
         <v>64</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>67</v>
-      </c>
-      <c r="F54" t="s">
-        <v>68</v>
       </c>
       <c r="G54">
         <v>102</v>
@@ -1635,11 +1578,8 @@
       <c r="D55" t="s">
         <v>64</v>
       </c>
-      <c r="E55" t="s">
-        <v>67</v>
-      </c>
       <c r="F55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G55">
         <v>169</v>

</xml_diff>